<commit_message>
update action to babiole and motd
</commit_message>
<xml_diff>
--- a/score_blank.xlsx
+++ b/score_blank.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="0" windowWidth="27855" windowHeight="13020"/>
+    <workbookView xWindow="5700" yWindow="0" windowWidth="27855" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="2" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Abandon</t>
   </si>
   <si>
-    <t>Echanges de points &amp; achats d'actions</t>
-  </si>
-  <si>
     <t>ROTD</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>Ligue été 2021 - GL AND HF !</t>
+  </si>
+  <si>
+    <t>Echanges de points &amp; babioles</t>
   </si>
 </sst>
 </file>
@@ -1119,12 +1119,57 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1164,30 +1209,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1195,27 +1216,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1502,7 +1502,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,48 +1517,48 @@
   <sheetData>
     <row r="1" spans="2:9" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="100" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="102"/>
+      <c r="B2" s="115" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="117"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="123" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="119"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="103" t="s">
+      <c r="F3" s="119"/>
+      <c r="G3" s="120" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122"/>
+    </row>
+    <row r="4" spans="2:9" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="124" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="125"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="118" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="106"/>
-      <c r="I3" s="107"/>
-    </row>
-    <row r="4" spans="2:9" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="109" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="103" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="106"/>
-      <c r="I4" s="107"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="120" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="121"/>
+      <c r="I4" s="122"/>
     </row>
     <row r="5" spans="2:9" s="2" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1581,9 +1581,9 @@
         <v>0</v>
       </c>
       <c r="D8" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="121"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="128"/>
       <c r="F8" s="61"/>
       <c r="G8" s="66"/>
       <c r="H8" s="66"/>
@@ -1597,9 +1597,9 @@
         <v>4</v>
       </c>
       <c r="D9" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="122"/>
+        <v>11</v>
+      </c>
+      <c r="E9" s="129"/>
       <c r="F9" s="45"/>
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
@@ -1613,42 +1613,42 @@
         <v>1</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="122"/>
+        <v>12</v>
+      </c>
+      <c r="E10" s="129"/>
       <c r="F10" s="45"/>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
       <c r="I10" s="41"/>
     </row>
     <row r="11" spans="2:9" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="130">
+      <c r="B11" s="101">
         <v>1</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="123"/>
+        <v>76</v>
+      </c>
+      <c r="E11" s="130"/>
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
       <c r="I11" s="51"/>
     </row>
     <row r="12" spans="2:9" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="127">
+      <c r="B12" s="98">
         <v>-2</v>
       </c>
-      <c r="C12" s="128" t="s">
+      <c r="C12" s="99" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="129" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="118" t="s">
-        <v>9</v>
+      <c r="E12" s="109" t="s">
+        <v>8</v>
       </c>
       <c r="F12" s="46"/>
       <c r="G12" s="39"/>
@@ -1660,12 +1660,12 @@
         <v>-1</v>
       </c>
       <c r="C13" s="77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="80" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="118"/>
+        <v>21</v>
+      </c>
+      <c r="E13" s="109"/>
       <c r="F13" s="46"/>
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
@@ -1676,12 +1676,12 @@
         <v>-4</v>
       </c>
       <c r="C14" s="77" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="118"/>
+        <v>17</v>
+      </c>
+      <c r="E14" s="109"/>
       <c r="F14" s="46"/>
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
@@ -1692,12 +1692,12 @@
         <v>-2</v>
       </c>
       <c r="C15" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="118"/>
+      <c r="E15" s="109"/>
       <c r="F15" s="46"/>
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
@@ -1708,12 +1708,12 @@
         <v>-2</v>
       </c>
       <c r="C16" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="118"/>
+      <c r="E16" s="109"/>
       <c r="F16" s="46"/>
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
@@ -1724,12 +1724,12 @@
         <v>-1</v>
       </c>
       <c r="C17" s="77" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="118"/>
+        <v>15</v>
+      </c>
+      <c r="E17" s="109"/>
       <c r="F17" s="46"/>
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
@@ -1740,12 +1740,12 @@
         <v>-2</v>
       </c>
       <c r="C18" s="77" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="80" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="118"/>
+        <v>13</v>
+      </c>
+      <c r="E18" s="109"/>
       <c r="F18" s="46"/>
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
@@ -1756,12 +1756,12 @@
         <v>-3</v>
       </c>
       <c r="C19" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="118"/>
+      <c r="E19" s="109"/>
       <c r="F19" s="46"/>
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
@@ -1772,12 +1772,12 @@
         <v>-2</v>
       </c>
       <c r="C20" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="118"/>
+      <c r="E20" s="109"/>
       <c r="F20" s="46"/>
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
@@ -1788,12 +1788,12 @@
         <v>-2</v>
       </c>
       <c r="C21" s="77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="118"/>
+        <v>33</v>
+      </c>
+      <c r="E21" s="109"/>
       <c r="F21" s="46"/>
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
@@ -1804,12 +1804,12 @@
         <v>-1</v>
       </c>
       <c r="C22" s="77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="80" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="118"/>
+        <v>14</v>
+      </c>
+      <c r="E22" s="109"/>
       <c r="F22" s="46"/>
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
@@ -1820,12 +1820,12 @@
         <v>-1</v>
       </c>
       <c r="C23" s="77" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="80" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="118"/>
+        <v>16</v>
+      </c>
+      <c r="E23" s="109"/>
       <c r="F23" s="46"/>
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
@@ -1836,12 +1836,12 @@
         <v>-1</v>
       </c>
       <c r="C24" s="77" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="118"/>
+      <c r="E24" s="109"/>
       <c r="F24" s="46"/>
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
@@ -1852,12 +1852,12 @@
         <v>-2</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" s="80" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="119"/>
+        <v>38</v>
+      </c>
+      <c r="E25" s="110"/>
       <c r="F25" s="46"/>
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
@@ -1868,13 +1868,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="120" t="s">
-        <v>10</v>
+      <c r="E26" s="111" t="s">
+        <v>9</v>
       </c>
       <c r="F26" s="42"/>
       <c r="G26" s="43"/>
@@ -1886,12 +1886,12 @@
         <v>1</v>
       </c>
       <c r="C27" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="80" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="118"/>
+      <c r="E27" s="109"/>
       <c r="F27" s="46"/>
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
@@ -1902,12 +1902,12 @@
         <v>2</v>
       </c>
       <c r="C28" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="80" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="118"/>
+      <c r="E28" s="109"/>
       <c r="F28" s="46"/>
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
@@ -1918,12 +1918,12 @@
         <v>2</v>
       </c>
       <c r="C29" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="118"/>
+      <c r="E29" s="109"/>
       <c r="F29" s="46"/>
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
@@ -1934,12 +1934,12 @@
         <v>1</v>
       </c>
       <c r="C30" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="118"/>
+      <c r="E30" s="109"/>
       <c r="F30" s="46"/>
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
@@ -1950,12 +1950,12 @@
         <v>1</v>
       </c>
       <c r="C31" s="77" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="118"/>
+        <v>77</v>
+      </c>
+      <c r="E31" s="109"/>
       <c r="F31" s="46"/>
       <c r="G31" s="39"/>
       <c r="H31" s="39"/>
@@ -1966,12 +1966,12 @@
         <v>1</v>
       </c>
       <c r="C32" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="80" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" s="118"/>
+      <c r="E32" s="109"/>
       <c r="F32" s="46"/>
       <c r="G32" s="39"/>
       <c r="H32" s="39"/>
@@ -1982,12 +1982,12 @@
         <v>1</v>
       </c>
       <c r="C33" s="77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" s="118"/>
+        <v>78</v>
+      </c>
+      <c r="E33" s="109"/>
       <c r="F33" s="46"/>
       <c r="G33" s="39"/>
       <c r="H33" s="39"/>
@@ -1998,12 +1998,12 @@
         <v>3</v>
       </c>
       <c r="C34" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="80" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="118"/>
+      <c r="E34" s="109"/>
       <c r="F34" s="46"/>
       <c r="G34" s="39"/>
       <c r="H34" s="39"/>
@@ -2014,12 +2014,12 @@
         <v>2</v>
       </c>
       <c r="C35" s="77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="118"/>
+        <v>83</v>
+      </c>
+      <c r="E35" s="109"/>
       <c r="F35" s="46"/>
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
@@ -2030,12 +2030,12 @@
         <v>2</v>
       </c>
       <c r="C36" s="82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D36" s="83" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="119"/>
+        <v>79</v>
+      </c>
+      <c r="E36" s="110"/>
       <c r="F36" s="46"/>
       <c r="G36" s="39"/>
       <c r="H36" s="39"/>
@@ -2047,13 +2047,13 @@
         <v>1</v>
       </c>
       <c r="C37" s="87" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37" s="88" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="124" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="E37" s="112" t="s">
+        <v>66</v>
       </c>
       <c r="F37" s="26"/>
       <c r="G37" s="27"/>
@@ -2066,12 +2066,12 @@
         <v>1</v>
       </c>
       <c r="C38" s="90" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D38" s="91" t="s">
-        <v>71</v>
-      </c>
-      <c r="E38" s="125"/>
+        <v>70</v>
+      </c>
+      <c r="E38" s="113"/>
       <c r="F38" s="9"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
@@ -2083,12 +2083,12 @@
         <v>1</v>
       </c>
       <c r="C39" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="91" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="125"/>
+      <c r="E39" s="113"/>
       <c r="F39" s="9"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
@@ -2100,12 +2100,12 @@
         <v>1</v>
       </c>
       <c r="C40" s="90" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="91" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" s="125"/>
+      <c r="E40" s="113"/>
       <c r="F40" s="9"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -2117,12 +2117,12 @@
         <v>1</v>
       </c>
       <c r="C41" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="91" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="125"/>
+      <c r="E41" s="113"/>
       <c r="F41" s="9"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
@@ -2134,12 +2134,12 @@
         <v>1</v>
       </c>
       <c r="C42" s="90" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" s="91" t="s">
-        <v>81</v>
-      </c>
-      <c r="E42" s="125"/>
+        <v>80</v>
+      </c>
+      <c r="E42" s="113"/>
       <c r="F42" s="9"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -2151,12 +2151,12 @@
         <v>1</v>
       </c>
       <c r="C43" s="90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D43" s="91" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" s="125"/>
+        <v>81</v>
+      </c>
+      <c r="E43" s="113"/>
       <c r="F43" s="9"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
@@ -2171,9 +2171,9 @@
         <v>2</v>
       </c>
       <c r="D44" s="94" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="126"/>
+        <v>82</v>
+      </c>
+      <c r="E44" s="114"/>
       <c r="F44" s="28"/>
       <c r="G44" s="29"/>
       <c r="H44" s="29"/>
@@ -2183,8 +2183,8 @@
       <c r="B45" s="37"/>
       <c r="C45" s="36"/>
       <c r="D45" s="33"/>
-      <c r="E45" s="113" t="s">
-        <v>8</v>
+      <c r="E45" s="104" t="s">
+        <v>7</v>
       </c>
       <c r="F45" s="62"/>
       <c r="G45" s="67"/>
@@ -2195,7 +2195,7 @@
       <c r="B46" s="37"/>
       <c r="C46" s="36"/>
       <c r="D46" s="33"/>
-      <c r="E46" s="113"/>
+      <c r="E46" s="104"/>
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
@@ -2205,17 +2205,17 @@
       <c r="B47" s="38"/>
       <c r="C47" s="54"/>
       <c r="D47" s="32"/>
-      <c r="E47" s="113"/>
+      <c r="E47" s="104"/>
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="11"/>
     </row>
     <row r="48" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="114" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="115"/>
+      <c r="B48" s="105" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="106"/>
       <c r="D48" s="34"/>
       <c r="E48" s="21"/>
       <c r="F48" s="63"/>
@@ -2224,8 +2224,8 @@
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="114"/>
-      <c r="C49" s="115"/>
+      <c r="B49" s="105"/>
+      <c r="C49" s="106"/>
       <c r="D49" s="34"/>
       <c r="E49" s="22"/>
       <c r="F49" s="64"/>
@@ -2234,8 +2234,8 @@
       <c r="I49" s="14"/>
     </row>
     <row r="50" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="105"/>
+      <c r="C50" s="106"/>
       <c r="D50" s="34"/>
       <c r="E50" s="22"/>
       <c r="F50" s="64"/>
@@ -2244,8 +2244,8 @@
       <c r="I50" s="14"/>
     </row>
     <row r="51" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="114"/>
-      <c r="C51" s="115"/>
+      <c r="B51" s="105"/>
+      <c r="C51" s="106"/>
       <c r="D51" s="34"/>
       <c r="E51" s="22"/>
       <c r="F51" s="64"/>
@@ -2254,8 +2254,8 @@
       <c r="I51" s="14"/>
     </row>
     <row r="52" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="114"/>
-      <c r="C52" s="115"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="106"/>
       <c r="D52" s="34"/>
       <c r="E52" s="22"/>
       <c r="F52" s="64"/>
@@ -2264,8 +2264,8 @@
       <c r="I52" s="14"/>
     </row>
     <row r="53" spans="2:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="116"/>
-      <c r="C53" s="117"/>
+      <c r="B53" s="107"/>
+      <c r="C53" s="108"/>
       <c r="D53" s="35"/>
       <c r="E53" s="23"/>
       <c r="F53" s="65"/>
@@ -2274,10 +2274,10 @@
       <c r="I53" s="16"/>
     </row>
     <row r="54" spans="2:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="111" t="s">
+      <c r="B54" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="112"/>
+      <c r="C54" s="127"/>
       <c r="D54" s="20"/>
       <c r="E54" s="24"/>
       <c r="F54" s="65"/>
@@ -2286,10 +2286,10 @@
       <c r="I54" s="16"/>
     </row>
     <row r="55" spans="2:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="98" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="99"/>
+      <c r="B55" s="102" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="103"/>
       <c r="D55" s="31"/>
       <c r="E55" s="25"/>
       <c r="F55" s="95"/>
@@ -2298,10 +2298,10 @@
       <c r="I55" s="96"/>
     </row>
     <row r="56" spans="2:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="98" t="s">
+      <c r="B56" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="99"/>
+      <c r="C56" s="103"/>
       <c r="D56" s="31"/>
       <c r="E56" s="25"/>
       <c r="F56" s="17"/>
@@ -2311,6 +2311,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="E45:E47"/>
     <mergeCell ref="B48:C53"/>
@@ -2318,15 +2326,7 @@
     <mergeCell ref="E26:E36"/>
     <mergeCell ref="E37:E44"/>
     <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="E8:E11"/>
   </mergeCells>
   <pageMargins left="0.30208333333333331" right="0.26041666666666669" top="0.32291666666666669" bottom="0.26041666666666669" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update orga AM après 1ere rencontre am, cfr update.md 16/06
</commit_message>
<xml_diff>
--- a/score_blank.xlsx
+++ b/score_blank.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="0" windowWidth="27855" windowHeight="13020"/>
+    <workbookView xWindow="7620" yWindow="0" windowWidth="27855" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Dernier debout </t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>Chercher dans son deck 3 fois durant le même tour</t>
+  </si>
+  <si>
+    <t>Non classé</t>
   </si>
 </sst>
 </file>
@@ -981,7 +984,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1155,82 +1158,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1256,7 +1184,85 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1540,10 +1546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,48 +1564,48 @@
   <sheetData>
     <row r="1" spans="2:9" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="117" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="87"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="119"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="88" t="s">
+      <c r="C3" s="121"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="89"/>
-      <c r="G3" s="90" t="s">
+      <c r="F3" s="121"/>
+      <c r="G3" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="91"/>
-      <c r="I3" s="92"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="124"/>
     </row>
     <row r="4" spans="2:9" s="1" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="95"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="88" t="s">
+      <c r="C4" s="115"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="89"/>
-      <c r="G4" s="90" t="s">
+      <c r="F4" s="121"/>
+      <c r="G4" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="91"/>
-      <c r="I4" s="92"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="124"/>
     </row>
     <row r="5" spans="2:9" s="2" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1624,13 +1630,13 @@
       <c r="D8" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="105" t="s">
+      <c r="E8" s="116" t="s">
         <v>85</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
-      <c r="I8" s="119"/>
+      <c r="I8" s="94"/>
     </row>
     <row r="9" spans="2:9" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="62">
@@ -1642,11 +1648,11 @@
       <c r="D9" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="103"/>
+      <c r="E9" s="106"/>
       <c r="F9" s="38"/>
       <c r="G9" s="35"/>
       <c r="H9" s="35"/>
-      <c r="I9" s="120"/>
+      <c r="I9" s="95"/>
     </row>
     <row r="10" spans="2:9" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="62">
@@ -1658,11 +1664,11 @@
       <c r="D10" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="103"/>
+      <c r="E10" s="106"/>
       <c r="F10" s="38"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="120"/>
+      <c r="I10" s="95"/>
     </row>
     <row r="11" spans="2:9" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="83">
@@ -1674,11 +1680,11 @@
       <c r="D11" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="104"/>
+      <c r="E11" s="107"/>
       <c r="F11" s="38"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="120"/>
+      <c r="I11" s="95"/>
     </row>
     <row r="12" spans="2:9" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="80">
@@ -1690,7 +1696,7 @@
       <c r="D12" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="103" t="s">
+      <c r="E12" s="106" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="38"/>
@@ -1708,7 +1714,7 @@
       <c r="D13" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="103"/>
+      <c r="E13" s="106"/>
       <c r="F13" s="38"/>
       <c r="G13" s="35"/>
       <c r="H13" s="35"/>
@@ -1724,7 +1730,7 @@
       <c r="D14" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="103"/>
+      <c r="E14" s="106"/>
       <c r="F14" s="38"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
@@ -1740,7 +1746,7 @@
       <c r="D15" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="103"/>
+      <c r="E15" s="106"/>
       <c r="F15" s="38"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
@@ -1756,7 +1762,7 @@
       <c r="D16" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="103"/>
+      <c r="E16" s="106"/>
       <c r="F16" s="38"/>
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
@@ -1772,7 +1778,7 @@
       <c r="D17" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="103"/>
+      <c r="E17" s="106"/>
       <c r="F17" s="38"/>
       <c r="G17" s="35"/>
       <c r="H17" s="35"/>
@@ -1788,7 +1794,7 @@
       <c r="D18" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="103"/>
+      <c r="E18" s="106"/>
       <c r="F18" s="38"/>
       <c r="G18" s="35"/>
       <c r="H18" s="35"/>
@@ -1804,7 +1810,7 @@
       <c r="D19" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="103"/>
+      <c r="E19" s="106"/>
       <c r="F19" s="38"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
@@ -1820,7 +1826,7 @@
       <c r="D20" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="103"/>
+      <c r="E20" s="106"/>
       <c r="F20" s="38"/>
       <c r="G20" s="35"/>
       <c r="H20" s="35"/>
@@ -1836,7 +1842,7 @@
       <c r="D21" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="103"/>
+      <c r="E21" s="106"/>
       <c r="F21" s="38"/>
       <c r="G21" s="35"/>
       <c r="H21" s="35"/>
@@ -1852,7 +1858,7 @@
       <c r="D22" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="103"/>
+      <c r="E22" s="106"/>
       <c r="F22" s="38"/>
       <c r="G22" s="35"/>
       <c r="H22" s="35"/>
@@ -1868,7 +1874,7 @@
       <c r="D23" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="103"/>
+      <c r="E23" s="106"/>
       <c r="F23" s="38"/>
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
@@ -1884,7 +1890,7 @@
       <c r="D24" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="103"/>
+      <c r="E24" s="106"/>
       <c r="F24" s="38"/>
       <c r="G24" s="35"/>
       <c r="H24" s="35"/>
@@ -1900,7 +1906,7 @@
       <c r="D25" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="104"/>
+      <c r="E25" s="107"/>
       <c r="F25" s="38"/>
       <c r="G25" s="35"/>
       <c r="H25" s="35"/>
@@ -1910,13 +1916,13 @@
       <c r="B26" s="61">
         <v>1</v>
       </c>
-      <c r="C26" s="112" t="s">
+      <c r="C26" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="113" t="s">
+      <c r="D26" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="103" t="s">
+      <c r="E26" s="106" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="38"/>
@@ -1934,7 +1940,7 @@
       <c r="D27" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="103"/>
+      <c r="E27" s="106"/>
       <c r="F27" s="38"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
@@ -1950,7 +1956,7 @@
       <c r="D28" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="103"/>
+      <c r="E28" s="106"/>
       <c r="F28" s="38"/>
       <c r="G28" s="35"/>
       <c r="H28" s="35"/>
@@ -1966,7 +1972,7 @@
       <c r="D29" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="103"/>
+      <c r="E29" s="106"/>
       <c r="F29" s="38"/>
       <c r="G29" s="35"/>
       <c r="H29" s="35"/>
@@ -1982,7 +1988,7 @@
       <c r="D30" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="103"/>
+      <c r="E30" s="106"/>
       <c r="F30" s="38"/>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
@@ -1998,7 +2004,7 @@
       <c r="D31" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="103"/>
+      <c r="E31" s="106"/>
       <c r="F31" s="38"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
@@ -2014,7 +2020,7 @@
       <c r="D32" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="103"/>
+      <c r="E32" s="106"/>
       <c r="F32" s="38"/>
       <c r="G32" s="35"/>
       <c r="H32" s="35"/>
@@ -2030,7 +2036,7 @@
       <c r="D33" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="103"/>
+      <c r="E33" s="106"/>
       <c r="F33" s="38"/>
       <c r="G33" s="35"/>
       <c r="H33" s="35"/>
@@ -2046,7 +2052,7 @@
       <c r="D34" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="103"/>
+      <c r="E34" s="106"/>
       <c r="F34" s="38"/>
       <c r="G34" s="35"/>
       <c r="H34" s="35"/>
@@ -2056,17 +2062,17 @@
       <c r="B35" s="83">
         <v>2</v>
       </c>
-      <c r="C35" s="114" t="s">
+      <c r="C35" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="115" t="s">
+      <c r="D35" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="104"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="122"/>
-      <c r="H35" s="122"/>
-      <c r="I35" s="123"/>
+      <c r="E35" s="107"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="98"/>
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42"/>
@@ -2079,7 +2085,7 @@
       <c r="D36" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="106" t="s">
+      <c r="E36" s="108" t="s">
         <v>62</v>
       </c>
       <c r="F36" s="23"/>
@@ -2098,7 +2104,7 @@
       <c r="D37" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="107"/>
+      <c r="E37" s="109"/>
       <c r="F37" s="9"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
@@ -2115,7 +2121,7 @@
       <c r="D38" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="107"/>
+      <c r="E38" s="109"/>
       <c r="F38" s="9"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
@@ -2132,7 +2138,7 @@
       <c r="D39" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="107"/>
+      <c r="E39" s="109"/>
       <c r="F39" s="9"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
@@ -2149,7 +2155,7 @@
       <c r="D40" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="107"/>
+      <c r="E40" s="109"/>
       <c r="F40" s="9"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -2166,7 +2172,7 @@
       <c r="D41" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="E41" s="107"/>
+      <c r="E41" s="109"/>
       <c r="F41" s="9"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
@@ -2183,7 +2189,7 @@
       <c r="D42" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="107"/>
+      <c r="E42" s="109"/>
       <c r="F42" s="9"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -2200,7 +2206,7 @@
       <c r="D43" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="E43" s="108"/>
+      <c r="E43" s="110"/>
       <c r="F43" s="25"/>
       <c r="G43" s="26"/>
       <c r="H43" s="26"/>
@@ -2210,7 +2216,7 @@
       <c r="B44" s="33"/>
       <c r="C44" s="32"/>
       <c r="D44" s="29"/>
-      <c r="E44" s="98" t="s">
+      <c r="E44" s="101" t="s">
         <v>7</v>
       </c>
       <c r="F44" s="46"/>
@@ -2222,7 +2228,7 @@
       <c r="B45" s="33"/>
       <c r="C45" s="32"/>
       <c r="D45" s="29"/>
-      <c r="E45" s="98"/>
+      <c r="E45" s="101"/>
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -2232,17 +2238,17 @@
       <c r="B46" s="34"/>
       <c r="C46" s="41"/>
       <c r="D46" s="28"/>
-      <c r="E46" s="98"/>
+      <c r="E46" s="101"/>
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="11"/>
     </row>
     <row r="47" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="99" t="s">
+      <c r="B47" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="100"/>
+      <c r="C47" s="103"/>
       <c r="D47" s="30"/>
       <c r="E47" s="18"/>
       <c r="F47" s="47"/>
@@ -2251,8 +2257,8 @@
       <c r="I47" s="13"/>
     </row>
     <row r="48" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="99"/>
-      <c r="C48" s="100"/>
+      <c r="B48" s="102"/>
+      <c r="C48" s="103"/>
       <c r="D48" s="30"/>
       <c r="E48" s="19"/>
       <c r="F48" s="48"/>
@@ -2261,8 +2267,8 @@
       <c r="I48" s="14"/>
     </row>
     <row r="49" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="99"/>
-      <c r="C49" s="100"/>
+      <c r="B49" s="102"/>
+      <c r="C49" s="103"/>
       <c r="D49" s="30"/>
       <c r="E49" s="19"/>
       <c r="F49" s="48"/>
@@ -2271,8 +2277,8 @@
       <c r="I49" s="14"/>
     </row>
     <row r="50" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="99"/>
-      <c r="C50" s="100"/>
+      <c r="B50" s="102"/>
+      <c r="C50" s="103"/>
       <c r="D50" s="30"/>
       <c r="E50" s="19"/>
       <c r="F50" s="48"/>
@@ -2281,8 +2287,8 @@
       <c r="I50" s="14"/>
     </row>
     <row r="51" spans="2:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="101"/>
-      <c r="C51" s="102"/>
+      <c r="B51" s="104"/>
+      <c r="C51" s="105"/>
       <c r="D51" s="31"/>
       <c r="E51" s="20"/>
       <c r="F51" s="49"/>
@@ -2291,10 +2297,10 @@
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="109" t="s">
+      <c r="B52" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="110"/>
+      <c r="C52" s="114"/>
       <c r="D52" s="17"/>
       <c r="E52" s="21"/>
       <c r="F52" s="49"/>
@@ -2302,11 +2308,11 @@
       <c r="H52" s="52"/>
       <c r="I52" s="15"/>
     </row>
-    <row r="53" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="96" t="s">
+    <row r="53" spans="2:9" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="97"/>
+      <c r="C53" s="112"/>
       <c r="D53" s="84"/>
       <c r="E53" s="22"/>
       <c r="F53" s="78"/>
@@ -2314,42 +2320,44 @@
       <c r="H53" s="16"/>
       <c r="I53" s="79"/>
     </row>
-    <row r="54" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="96" t="s">
+    <row r="54" spans="2:9" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="97"/>
-      <c r="D54" s="84"/>
+      <c r="C54" s="112"/>
+      <c r="D54" s="85"/>
       <c r="E54" s="22"/>
       <c r="F54" s="78"/>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
       <c r="I54" s="79"/>
     </row>
-    <row r="55" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="94" t="s">
+    <row r="55" spans="2:9" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="111" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="112"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="78"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="79"/>
+    </row>
+    <row r="56" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="99" t="s">
         <v>84</v>
       </c>
-      <c r="C55" s="124"/>
-      <c r="D55" s="124"/>
-      <c r="E55" s="95"/>
-      <c r="F55" s="116"/>
-      <c r="G55" s="117"/>
-      <c r="H55" s="117"/>
-      <c r="I55" s="118"/>
+      <c r="C56" s="100"/>
+      <c r="D56" s="100"/>
+      <c r="E56" s="115"/>
+      <c r="F56" s="91"/>
+      <c r="G56" s="92"/>
+      <c r="H56" s="92"/>
+      <c r="I56" s="93"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="B47:C51"/>
-    <mergeCell ref="E12:E25"/>
-    <mergeCell ref="E26:E35"/>
-    <mergeCell ref="E36:E43"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D55:E55"/>
+  <mergeCells count="19">
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="E3:F3"/>
@@ -2358,6 +2366,17 @@
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="B47:C51"/>
+    <mergeCell ref="E12:E25"/>
+    <mergeCell ref="E26:E35"/>
+    <mergeCell ref="E36:E43"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="B54:C54"/>
   </mergeCells>
   <pageMargins left="0.30208333333333331" right="0.26041666666666669" top="0.32291666666666669" bottom="0.26041666666666669" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>